<commit_message>
start before cleaning the data
</commit_message>
<xml_diff>
--- a/resubmision/kliceni_proklicovani_klima.xlsx
+++ b/resubmision/kliceni_proklicovani_klima.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="kliceni" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="40">
   <si>
     <t>no1</t>
   </si>
@@ -120,6 +120,21 @@
   </si>
   <si>
     <t>celkem</t>
+  </si>
+  <si>
+    <t>seed_n</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>dish</t>
+  </si>
+  <si>
+    <t>locality</t>
+  </si>
+  <si>
+    <t>date</t>
   </si>
 </sst>
 </file>
@@ -462,13 +477,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R23"/>
+  <dimension ref="A1:R49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R23" sqref="R23"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="17" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B1" s="1">
@@ -1775,6 +1793,265 @@
       <c r="R23">
         <f t="shared" si="0"/>
         <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>39</v>
+      </c>
+      <c r="C27" t="s">
+        <v>37</v>
+      </c>
+      <c r="D27" t="s">
+        <v>35</v>
+      </c>
+      <c r="E27" t="s">
+        <v>36</v>
+      </c>
+      <c r="F27" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B28" s="1">
+        <v>42016</v>
+      </c>
+      <c r="C28" t="s">
+        <v>16</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B29" s="1">
+        <v>42016</v>
+      </c>
+      <c r="C29" t="s">
+        <v>17</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B30" s="1">
+        <v>42016</v>
+      </c>
+      <c r="C30" t="s">
+        <v>18</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B31" s="1">
+        <v>42016</v>
+      </c>
+      <c r="C31" t="s">
+        <v>19</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B32" s="1">
+        <v>42016</v>
+      </c>
+      <c r="C32" t="s">
+        <v>33</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B33" s="1">
+        <v>42016</v>
+      </c>
+      <c r="C33" t="s">
+        <v>20</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B34" s="1">
+        <v>42016</v>
+      </c>
+      <c r="C34" t="s">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B35" s="1">
+        <v>42016</v>
+      </c>
+      <c r="C35" t="s">
+        <v>1</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B36" s="1">
+        <v>42016</v>
+      </c>
+      <c r="C36" t="s">
+        <v>2</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B37" s="1">
+        <v>42016</v>
+      </c>
+      <c r="C37" t="s">
+        <v>3</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B38" s="1">
+        <v>42016</v>
+      </c>
+      <c r="C38" t="s">
+        <v>4</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B39" s="1">
+        <v>42016</v>
+      </c>
+      <c r="C39" t="s">
+        <v>5</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B40" s="1">
+        <v>42016</v>
+      </c>
+      <c r="C40" t="s">
+        <v>6</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B41" s="1">
+        <v>42016</v>
+      </c>
+      <c r="C41" t="s">
+        <v>7</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B42" s="1">
+        <v>42016</v>
+      </c>
+      <c r="C42" t="s">
+        <v>8</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B43" s="1">
+        <v>42016</v>
+      </c>
+      <c r="C43" t="s">
+        <v>9</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B44" s="1">
+        <v>42016</v>
+      </c>
+      <c r="C44" t="s">
+        <v>10</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B45" s="1">
+        <v>42016</v>
+      </c>
+      <c r="C45" t="s">
+        <v>11</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B46" s="1">
+        <v>42016</v>
+      </c>
+      <c r="C46" t="s">
+        <v>12</v>
+      </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B47" s="1">
+        <v>42016</v>
+      </c>
+      <c r="C47" t="s">
+        <v>13</v>
+      </c>
+      <c r="D47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B48" s="1">
+        <v>42016</v>
+      </c>
+      <c r="C48" t="s">
+        <v>14</v>
+      </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B49" s="1">
+        <v>42016</v>
+      </c>
+      <c r="C49" t="s">
+        <v>15</v>
+      </c>
+      <c r="D49">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1787,10 +2064,13 @@
   <dimension ref="A1:R13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R8" sqref="R8"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="17" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B1" s="1">

</xml_diff>